<commit_message>
Adding my data to the file
</commit_message>
<xml_diff>
--- a/Data for Project One.csv.xlsx
+++ b/Data for Project One.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\project_one\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0B6702-B4C7-4994-A4D7-276FD0BF92B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B659C74-4081-4606-95EA-4E29B6A7895A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5CFF1D6-3364-470A-867C-3C3C06224521}"/>
+    <workbookView xWindow="41550" yWindow="5505" windowWidth="15375" windowHeight="7875" xr2:uid="{F5CFF1D6-3364-470A-867C-3C3C06224521}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
   <si>
     <t>State</t>
   </si>
@@ -504,14 +504,44 @@
     <t>No. of Officers</t>
   </si>
   <si>
-    <t>No. of (Offenses</t>
+    <t>No. of (Burglary)</t>
+  </si>
+  <si>
+    <t>No. of Non-Violent Crimes</t>
+  </si>
+  <si>
+    <t>NJ0111100</t>
+  </si>
+  <si>
+    <t>NM0260100</t>
+  </si>
+  <si>
+    <t>NY0010100</t>
+  </si>
+  <si>
+    <t>NC0920100</t>
+  </si>
+  <si>
+    <t>ND0080100</t>
+  </si>
+  <si>
+    <t>OHCOP0000</t>
+  </si>
+  <si>
+    <t>OK0550400</t>
+  </si>
+  <si>
+    <t>OR0240200</t>
+  </si>
+  <si>
+    <t>PA0220200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,6 +589,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -581,7 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -593,12 +628,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <font>
         <strike val="0"/>
@@ -608,36 +647,12 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -677,6 +692,26 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -699,6 +734,26 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -800,16 +855,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48E33B0E-90C7-43C2-98B8-028A598D2217}" name="Table1" displayName="Table1" ref="A1:G51" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:G51" xr:uid="{6534F8AF-F9D2-4EA8-8455-068E982FC994}"/>
-  <tableColumns count="7">
-    <tableColumn id="5" xr3:uid="{81237C52-AF75-4CFC-8494-43A3B5B48997}" name="State" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{56ADF8B3-8736-4E8D-A188-DA3976CBC2C2}" name="State Ab." dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{1D6BB7B1-3ABC-4DE0-8C6F-43587D74CBF0}" name="State Capital" dataDxfId="6" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{45D2817E-DC79-40C1-A1EA-04CC9851FB0C}" name="Population" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{FD7846DE-B7E2-4920-8904-903117FED95A}" name="ORI Code" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{48E33B0E-90C7-43C2-98B8-028A598D2217}" name="Table1" displayName="Table1" ref="A1:H51" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H51" xr:uid="{6534F8AF-F9D2-4EA8-8455-068E982FC994}"/>
+  <tableColumns count="8">
+    <tableColumn id="5" xr3:uid="{81237C52-AF75-4CFC-8494-43A3B5B48997}" name="State" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{56ADF8B3-8736-4E8D-A188-DA3976CBC2C2}" name="State Ab." dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1D6BB7B1-3ABC-4DE0-8C6F-43587D74CBF0}" name="State Capital" dataDxfId="5" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{45D2817E-DC79-40C1-A1EA-04CC9851FB0C}" name="Population" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{FD7846DE-B7E2-4920-8904-903117FED95A}" name="ORI Code" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{E7DA3915-0208-45D4-810E-F796221A5692}" name="No. of Officers" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{D941BB4B-D99F-4BA9-876C-85FD63EF27EE}" name="No. of (Offenses" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{D941BB4B-D99F-4BA9-876C-85FD63EF27EE}" name="No. of (Burglary)" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{420A4049-018A-4791-A909-AEA304077793}" name="No. of Non-Violent Crimes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1112,25 +1168,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3B1FE12-01C4-4052-96C1-EACE650E7C23}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="6" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="7" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="26.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1143,7 +1200,7 @@
       <c r="D1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>154</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1152,8 +1209,11 @@
       <c r="G1" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
@@ -1167,7 +1227,7 @@
         <v>198525</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>101</v>
       </c>
@@ -1181,7 +1241,7 @@
         <v>32113</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -1195,7 +1255,7 @@
         <v>1680992</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>104</v>
       </c>
@@ -1209,7 +1269,7 @@
         <v>197312</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>105</v>
       </c>
@@ -1223,7 +1283,7 @@
         <v>513624</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>106</v>
       </c>
@@ -1237,7 +1297,7 @@
         <v>727211</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
@@ -1251,7 +1311,7 @@
         <v>122105</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>108</v>
       </c>
@@ -1265,7 +1325,7 @@
         <v>38079</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>109</v>
       </c>
@@ -1279,7 +1339,7 @@
         <v>194500</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>110</v>
       </c>
@@ -1293,7 +1353,7 @@
         <v>506811</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>111</v>
       </c>
@@ -1307,7 +1367,7 @@
         <v>345064</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>112</v>
       </c>
@@ -1321,7 +1381,7 @@
         <v>228959</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>113</v>
       </c>
@@ -1335,7 +1395,7 @@
         <v>114230</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>114</v>
       </c>
@@ -1349,7 +1409,7 @@
         <v>876384</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>115</v>
       </c>
@@ -1363,7 +1423,7 @@
         <v>214237</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>116</v>
       </c>
@@ -1377,7 +1437,7 @@
         <v>125310</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>117</v>
       </c>
@@ -1391,7 +1451,7 @@
         <v>27679</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>118</v>
       </c>
@@ -1405,7 +1465,7 @@
         <v>220236</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>119</v>
       </c>
@@ -1419,7 +1479,7 @@
         <v>18681</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>120</v>
       </c>
@@ -1433,7 +1493,7 @@
         <v>39174</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>121</v>
       </c>
@@ -1447,7 +1507,7 @@
         <v>692600</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
@@ -1461,7 +1521,7 @@
         <v>118210</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>123</v>
       </c>
@@ -1475,7 +1535,7 @@
         <v>308096</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>124</v>
       </c>
@@ -1489,7 +1549,7 @@
         <v>160628</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>125</v>
       </c>
@@ -1503,7 +1563,7 @@
         <v>42838</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>126</v>
       </c>
@@ -1517,7 +1577,7 @@
         <v>32315</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>127</v>
       </c>
@@ -1531,7 +1591,7 @@
         <v>289102</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>128</v>
       </c>
@@ -1545,7 +1605,7 @@
         <v>55916</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>129</v>
       </c>
@@ -1559,7 +1619,7 @@
         <v>43627</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>130</v>
       </c>
@@ -1572,8 +1632,11 @@
       <c r="D31" s="5">
         <v>83203</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>131</v>
       </c>
@@ -1586,8 +1649,11 @@
       <c r="D32" s="5">
         <v>84683</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>132</v>
       </c>
@@ -1600,8 +1666,11 @@
       <c r="D33" s="5">
         <v>96460</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>133</v>
       </c>
@@ -1614,8 +1683,11 @@
       <c r="D34" s="5">
         <v>474069</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>134</v>
       </c>
@@ -1628,8 +1700,11 @@
       <c r="D35" s="5">
         <v>73529</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>135</v>
       </c>
@@ -1642,8 +1717,11 @@
       <c r="D36" s="5">
         <v>898553</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E36" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="24" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>136</v>
       </c>
@@ -1656,8 +1734,11 @@
       <c r="D37" s="5">
         <v>655057</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>137</v>
       </c>
@@ -1670,8 +1751,11 @@
       <c r="D38" s="5">
         <v>174365</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>138</v>
       </c>
@@ -1684,8 +1768,11 @@
       <c r="D39" s="5">
         <v>49528</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>139</v>
       </c>
@@ -1698,8 +1785,9 @@
       <c r="D40" s="5">
         <v>179883</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>140</v>
       </c>
@@ -1713,7 +1801,7 @@
         <v>131674</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>141</v>
       </c>
@@ -1727,7 +1815,7 @@
         <v>13646</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>142</v>
       </c>
@@ -1741,7 +1829,7 @@
         <v>670820</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
         <v>143</v>
       </c>
@@ -1755,7 +1843,7 @@
         <v>978908</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>144</v>
       </c>
@@ -1769,7 +1857,7 @@
         <v>200567</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>145</v>
       </c>
@@ -1783,7 +1871,7 @@
         <v>7855</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
         <v>146</v>
       </c>
@@ -1797,7 +1885,7 @@
         <v>230436</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
         <v>148</v>
       </c>
@@ -1811,7 +1899,7 @@
         <v>46478</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>149</v>
       </c>
@@ -1825,7 +1913,7 @@
         <v>46536</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>150</v>
       </c>
@@ -1839,7 +1927,7 @@
         <v>259680</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>151</v>
       </c>
@@ -1870,7 +1958,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>